<commit_message>
CNH market working verision
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/CNH_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/CNH_MainChecks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="18855" windowHeight="11250"/>
+    <workbookView xWindow="20385" yWindow="-15" windowWidth="10230" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="MainChecks" sheetId="2" r:id="rId1"/>
@@ -16,11 +16,11 @@
     <definedName name="AllTriggers">MainChecks!$I$5:$I$5</definedName>
     <definedName name="Currency">MainChecks!$B$1</definedName>
     <definedName name="EvaluationDate">MainChecks!$C$3</definedName>
-    <definedName name="FirstIndex">MainChecks!$B$11</definedName>
+    <definedName name="FirstIndex">MainChecks!$B$8</definedName>
     <definedName name="InterestRatesTrigger">MainChecks!$I$5</definedName>
-    <definedName name="SecondIMMDate">MainChecks!$C$12</definedName>
+    <definedName name="SecondIMMDate">MainChecks!$C$9</definedName>
     <definedName name="Trigger">MainChecks!$I$2</definedName>
-    <definedName name="Yesterday">MainChecks!$C$9</definedName>
+    <definedName name="Yesterday">MainChecks!$C$6</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -74,10 +74,10 @@
     <t>Eikon</t>
   </si>
   <si>
-    <t>Stale</t>
+    <t>CNH</t>
   </si>
   <si>
-    <t>CNH</t>
+    <t>z</t>
   </si>
 </sst>
 </file>
@@ -189,7 +189,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -566,6 +566,17 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -694,11 +705,9 @@
     <xf numFmtId="170" fontId="7" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="8" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="6" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="1"/>
@@ -793,9 +802,9 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 10:47:16</v>
+        <v>Updated at 17:23:41</v>
         <stp/>
-        <stp>{00B14CD1-E74C-457F-98D5-DFB4AB1EF186}</stp>
+        <stp>{23F73E56-4374-4521-A019-F56B0FDDA292}</stp>
         <tr r="I3" s="2"/>
       </tp>
     </main>
@@ -903,31 +912,11 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="General Settings"/>
-      <sheetName val="Libor"/>
-      <sheetName val="LiborSwapIsdaFixAm"/>
-      <sheetName val="LiborSwapForBasisCalc"/>
-      <sheetName val="LiborSwapIsdaFixPm"/>
-      <sheetName val="BasisSwap1MxM"/>
-      <sheetName val="BasisSwap3M6M"/>
-      <sheetName val="BasisSwapxM12M"/>
+      <sheetName val="CNH Hibor"/>
       <sheetName val="Deposits"/>
       <sheetName val="FRA"/>
-      <sheetName val="Futures1M"/>
-      <sheetName val="Futures3M"/>
-      <sheetName val="ImmFra6M "/>
-      <sheetName val="FuturesHWConvAdj"/>
       <sheetName val="OIS"/>
-      <sheetName val="Swaps1M"/>
-      <sheetName val="SwapsIMMDated"/>
       <sheetName val="Swap3M"/>
-      <sheetName val="Swap6M"/>
-      <sheetName val="ON"/>
-      <sheetName val="1M (2)"/>
-      <sheetName val="3M (2)"/>
-      <sheetName val="FwdEONIAOIS"/>
-      <sheetName val="SFIX3"/>
-      <sheetName val="IB365"/>
-      <sheetName val="IBOR"/>
     </sheetNames>
     <definedNames>
       <definedName name="TriggerCounter" refersTo="='General Settings'!$D$7"/>
@@ -936,164 +925,42 @@
       <sheetData sheetId="0">
         <row r="7">
           <cell r="D7">
-            <v>2</v>
+            <v>19</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1">
+        <row r="6">
+          <cell r="K6" t="str">
+            <v>CnhHiborON#0001</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="2">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>3M</v>
+        <row r="4">
+          <cell r="E4" t="str">
+            <v>CNHOND_Quote#0001</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="3">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>Fwd Curve</v>
+        <row r="3">
+          <cell r="E3" t="str">
+            <v>CNHT1F1_Quote#0001</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="4">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>3M</v>
+        <row r="5">
+          <cell r="F5" t="str">
+            <v>CNHOISSW_Quote#0001</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="5">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>1L</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>3L</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="7">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>3L</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="8">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>USDSND_Quote#0000</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="9">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>USD1x4F_Quote</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="10">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>Q4</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="11">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>Q4</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="12">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>X4</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>3W</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="15">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>X1S</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="16">
-        <row r="7">
-          <cell r="D7">
-            <v>12</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="17">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>3L</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="18">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>6L</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>3L</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="21">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>6L</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="22">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>2X</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="23">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>USD-4Y=</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="24">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>USD-SWD=</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="25">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>USD-SWD=</v>
+        <row r="5">
+          <cell r="F5" t="str">
+            <v>CNHQM3H6M_Quote#0001</v>
           </cell>
         </row>
       </sheetData>
@@ -1400,13 +1267,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" style="5" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="2.28515625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" style="5" customWidth="1"/>
     <col min="8" max="8" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="2.85546875" style="5" customWidth="1"/>
@@ -1416,7 +1283,7 @@
     <row r="1" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="2" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
@@ -1458,7 +1325,7 @@
       <c r="F2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="11"/>
+      <c r="G2" s="52"/>
       <c r="H2" s="12" t="s">
         <v>3</v>
       </c>
@@ -1484,9 +1351,9 @@
         <f>UPPER(Currency)&amp;"STD"</f>
         <v>CNHSTD</v>
       </c>
-      <c r="C3" s="48" t="e">
+      <c r="C3" s="48">
         <f>_xll.qlCalendarAdjust(_xll.qlIndexFixingCalendar(FirstIndex),_xll.qlSettingsEvaluationDate(ISERROR(Trigger)),"f")</f>
-        <v>#VALUE!</v>
+        <v>41809</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="17" t="e">
@@ -1495,15 +1362,15 @@
       </c>
       <c r="F3" s="18" t="str">
         <f ca="1">IF(ISERROR(C3),_xll.ohRangeRetrieveError(C3),_xll.ohRangeRetrieveError(E3))</f>
-        <v/>
-      </c>
-      <c r="G3" s="11"/>
+        <v>qlYieldTSDiscount - ObjectHandler error: attempt to retrieve object with unknown ID 'CNHSTD'</v>
+      </c>
+      <c r="G3" s="52"/>
       <c r="H3" s="46" t="s">
         <v>14</v>
       </c>
       <c r="I3" s="45" t="str">
         <f>_xll.RData(H4,"LAST",,"FRQ:1S",,I4)</f>
-        <v>Updated at 10:47:16</v>
+        <v>Updated at 17:23:41</v>
       </c>
       <c r="J3" s="13"/>
       <c r="K3" s="4"/>
@@ -1526,9 +1393,9 @@
         <f>UPPER(Currency)&amp;"ON"</f>
         <v>CNHON</v>
       </c>
-      <c r="C4" s="40" t="e">
+      <c r="C4" s="40">
         <f>EvaluationDate</f>
-        <v>#VALUE!</v>
+        <v>41809</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="17" t="e">
@@ -1537,14 +1404,14 @@
       </c>
       <c r="F4" s="18" t="str">
         <f ca="1">IF(ISERROR(C4),_xll.ohRangeRetrieveError(C4),_xll.ohRangeRetrieveError(E4))</f>
-        <v/>
-      </c>
-      <c r="G4" s="11"/>
+        <v>qlYieldTSDiscount - ObjectHandler error: attempt to retrieve object with unknown ID 'CNHON'</v>
+      </c>
+      <c r="G4" s="52"/>
       <c r="H4" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="44" t="s">
-        <v>15</v>
+      <c r="I4" s="44">
+        <v>124.515625</v>
       </c>
       <c r="J4" s="13"/>
       <c r="K4" s="4"/>
@@ -1564,12 +1431,12 @@
     <row r="5" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="15" t="str">
-        <f>UPPER(Currency)&amp;"1M"</f>
-        <v>CNH1M</v>
+        <f>UPPER(Currency)&amp;"3M"</f>
+        <v>CNH3M</v>
       </c>
       <c r="C5" s="40" t="e">
-        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D","Following")</f>
-        <v>#VALUE!</v>
+        <f>#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="17" t="e">
@@ -1578,15 +1445,15 @@
       </c>
       <c r="F5" s="18" t="str">
         <f ca="1">IF(ISERROR(C5),_xll.ohRangeRetrieveError(C5),_xll.ohRangeRetrieveError(E5))</f>
-        <v>qlInterestRateIndexFixingDays - ObjectHandler error: attempt to retrieve object with unknown ID 'CnhLibor3M'</v>
-      </c>
-      <c r="G5" s="11"/>
+        <v/>
+      </c>
+      <c r="G5" s="52"/>
       <c r="H5" s="19" t="s">
         <v>13</v>
       </c>
       <c r="I5" s="20">
         <f>[1]!TriggerCounter</f>
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="J5" s="13"/>
       <c r="K5" s="4"/>
@@ -1605,30 +1472,27 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
-      <c r="B6" s="15" t="str">
-        <f>UPPER(Currency)&amp;"3M"</f>
-        <v>CNH3M</v>
-      </c>
-      <c r="C6" s="40" t="e">
-        <f>C5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="17" t="e">
-        <f>_xll.qlYieldTSDiscount(B6,C6,,Trigger)</f>
+      <c r="B6" s="23"/>
+      <c r="C6" s="41">
+        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-2D","Preceding")</f>
+        <v>41807</v>
+      </c>
+      <c r="D6" s="24"/>
+      <c r="E6" s="25" t="e">
+        <f>_xll.qlIndexFixing(FirstIndex,C6)</f>
         <v>#NUM!</v>
       </c>
-      <c r="F6" s="18" t="str">
+      <c r="F6" s="14" t="str">
         <f ca="1">IF(ISERROR(C6),_xll.ohRangeRetrieveError(C6),_xll.ohRangeRetrieveError(E6))</f>
-        <v/>
-      </c>
-      <c r="G6" s="11"/>
+        <v>qlIndexFixing - Missing HiborSN Actual/365 (Fixed) fixing for June 17th, 2014</v>
+      </c>
+      <c r="G6" s="52"/>
       <c r="H6" s="19" t="s">
         <v>4</v>
       </c>
       <c r="I6" s="20">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>735</v>
+        <v>159</v>
       </c>
       <c r="J6" s="13"/>
       <c r="K6" s="4"/>
@@ -1647,24 +1511,21 @@
     </row>
     <row r="7" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
-      <c r="B7" s="15" t="str">
-        <f>UPPER(Currency)&amp;"6M"</f>
-        <v>CNH6M</v>
-      </c>
-      <c r="C7" s="40" t="e">
-        <f>C6</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="17" t="e">
-        <f>_xll.qlYieldTSDiscount(B7,C7,,Trigger)</f>
+      <c r="B7" s="26"/>
+      <c r="C7" s="42">
+        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-1D","Preceding")</f>
+        <v>41808</v>
+      </c>
+      <c r="D7" s="35"/>
+      <c r="E7" s="28" t="e">
+        <f>_xll.qlIndexFixing(FirstIndex,C7)</f>
         <v>#NUM!</v>
       </c>
       <c r="F7" s="18" t="str">
         <f ca="1">IF(ISERROR(C7),_xll.ohRangeRetrieveError(C7),_xll.ohRangeRetrieveError(E7))</f>
-        <v/>
-      </c>
-      <c r="G7" s="11"/>
+        <v>qlIndexFixing - Missing HiborSN Actual/365 (Fixed) fixing for June 18th, 2014</v>
+      </c>
+      <c r="G7" s="52"/>
       <c r="H7" s="33" t="s">
         <v>7</v>
       </c>
@@ -1686,26 +1547,26 @@
       <c r="V7" s="4"/>
       <c r="W7" s="4"/>
     </row>
-    <row r="8" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
-      <c r="B8" s="15" t="str">
-        <f>UPPER(Currency)&amp;"1Y"</f>
-        <v>CNH1Y</v>
-      </c>
-      <c r="C8" s="40" t="e">
-        <f>C7</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="17" t="e">
-        <f>_xll.qlYieldTSDiscount(B8,C8,,Trigger)</f>
-        <v>#NUM!</v>
+      <c r="B8" s="26" t="str">
+        <f>PROPER(Currency)&amp;"Hibor3M"</f>
+        <v>CnhHibor3M</v>
+      </c>
+      <c r="C8" s="42">
+        <f>EvaluationDate</f>
+        <v>41809</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28">
+        <f>_xll.qlIndexFixing(FirstIndex,C8)</f>
+        <v>3.0844999999999997E-2</v>
       </c>
       <c r="F8" s="18" t="str">
-        <f ca="1">IF(ISERROR(C8),_xll.ohRangeRetrieveError(C8),_xll.ohRangeRetrieveError(E8))</f>
+        <f>IF(ISERROR(C8),_xll.ohRangeRetrieveError(C8),_xll.ohRangeRetrieveError(E8))</f>
         <v/>
       </c>
-      <c r="G8" s="11"/>
+      <c r="G8" s="52"/>
       <c r="H8" s="19" t="s">
         <v>8</v>
       </c>
@@ -1728,23 +1589,23 @@
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="41" t="e">
-        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-2D","Preceding")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25" t="e">
-        <f>_xll.qlIndexFixing(FirstIndex,C9)</f>
+      <c r="B9" s="29"/>
+      <c r="C9" s="43">
+        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),_xll.qlIMMNextDate(_xll.qlIMMNextDate(EvaluationDate+1)+1),-_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D")</f>
+        <v>41988</v>
+      </c>
+      <c r="D9" s="30"/>
+      <c r="E9" s="31" t="e">
+        <f>_xll.qlIndexFixing(FirstIndex,C9,TRUE)</f>
         <v>#NUM!</v>
       </c>
-      <c r="F9" s="14" t="str">
+      <c r="F9" s="32" t="str">
         <f ca="1">IF(ISERROR(C9),_xll.ohRangeRetrieveError(C9),_xll.ohRangeRetrieveError(E9))</f>
-        <v>qlIndexFixingCalendar - ObjectHandler error: attempt to retrieve object with unknown ID 'CnhLibor3M'</v>
-      </c>
-      <c r="G9" s="11"/>
+        <v>qlIndexFixing - null term structure set to this instance of HiborSN Actual/365 (Fixed)</v>
+      </c>
+      <c r="G9" s="52"/>
       <c r="H9" s="21" t="s">
         <v>9</v>
       </c>
@@ -1769,20 +1630,11 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="42" t="e">
-        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-1D","Preceding")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D10" s="35"/>
-      <c r="E10" s="28" t="e">
-        <f>_xll.qlIndexFixing(FirstIndex,C10)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F10" s="18" t="str">
-        <f ca="1">IF(ISERROR(C10),_xll.ohRangeRetrieveError(C10),_xll.ohRangeRetrieveError(E10))</f>
-        <v>qlIndexFixingCalendar - ObjectHandler error: attempt to retrieve object with unknown ID 'CnhLibor3M'</v>
-      </c>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
       <c r="G10" s="11"/>
       <c r="H10" s="21" t="s">
         <v>10</v>
@@ -1808,23 +1660,11 @@
     </row>
     <row r="11" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
-      <c r="B11" s="26" t="str">
-        <f>PROPER(Currency)&amp;IF(UPPER(Currency)="EUR","",IF(UPPER(Currency)="HKD","H","L"))&amp;"ibor3M"</f>
-        <v>CnhLibor3M</v>
-      </c>
-      <c r="C11" s="42" t="e">
-        <f>EvaluationDate</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="28" t="e">
-        <f>_xll.qlIndexFixing(FirstIndex,C11)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F11" s="18" t="str">
-        <f ca="1">IF(ISERROR(C11),_xll.ohRangeRetrieveError(C11),_xll.ohRangeRetrieveError(E11))</f>
-        <v/>
-      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="33" t="s">
         <v>11</v>
@@ -1848,25 +1688,16 @@
       <c r="V11" s="4"/>
       <c r="W11" s="4"/>
     </row>
-    <row r="12" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="43" t="e">
-        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),_xll.qlIMMNextDate(_xll.qlIMMNextDate(EvaluationDate+1)+1),-_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D")</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D12" s="30"/>
-      <c r="E12" s="31" t="e">
-        <f>_xll.qlIndexFixing(FirstIndex,C12,TRUE)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="F12" s="32" t="str">
-        <f ca="1">IF(ISERROR(C12),_xll.ohRangeRetrieveError(C12),_xll.ohRangeRetrieveError(E12))</f>
-        <v>qlInterestRateIndexFixingDays - ObjectHandler error: attempt to retrieve object with unknown ID 'CnhLibor3M'</v>
-      </c>
-      <c r="G12" s="51"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="52"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
       <c r="J12" s="13"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
@@ -2191,7 +2022,9 @@
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
+      <c r="I25" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
@@ -2859,11 +2692,6 @@
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="4"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
@@ -2884,11 +2712,6 @@
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
-      <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
@@ -2909,11 +2732,6 @@
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>

</xml_diff>

<commit_message>
CNH framework - 3M Curve
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/CNH_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/CNH_MainChecks.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>ObjectID</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>Stale</t>
   </si>
 </sst>
 </file>
@@ -802,9 +805,9 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 17:23:41</v>
+        <v>Updated at 16:44:19</v>
         <stp/>
-        <stp>{23F73E56-4374-4521-A019-F56B0FDDA292}</stp>
+        <stp>{58001B47-ADBF-4A31-B78B-F031D5961002}</stp>
         <tr r="I3" s="2"/>
       </tp>
     </main>
@@ -914,7 +917,7 @@
       <sheetName val="General Settings"/>
       <sheetName val="CNH Hibor"/>
       <sheetName val="Deposits"/>
-      <sheetName val="FRA"/>
+      <sheetName val="FRAs"/>
       <sheetName val="OIS"/>
       <sheetName val="Swap3M"/>
     </sheetNames>
@@ -925,42 +928,42 @@
       <sheetData sheetId="0">
         <row r="7">
           <cell r="D7">
-            <v>19</v>
+            <v>1</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
-        <row r="6">
-          <cell r="K6" t="str">
-            <v>CnhHiborON#0001</v>
+        <row r="7">
+          <cell r="D7">
+            <v>2</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="2">
-        <row r="4">
-          <cell r="E4" t="str">
-            <v>CNHOND_Quote#0001</v>
+        <row r="7">
+          <cell r="D7" t="str">
+            <v>CNHSWD_Quote</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="3">
-        <row r="3">
-          <cell r="E3" t="str">
-            <v>CNHT1F1_Quote#0001</v>
+        <row r="7">
+          <cell r="D7" t="str">
+            <v>CNH1x4F_Quote</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="4">
-        <row r="5">
-          <cell r="F5" t="str">
-            <v>CNHOISSW_Quote#0001</v>
+        <row r="7">
+          <cell r="D7" t="str">
+            <v>3W</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="5">
-        <row r="5">
-          <cell r="F5" t="str">
-            <v>CNHQM3H6M_Quote#0001</v>
+        <row r="7">
+          <cell r="D7" t="str">
+            <v>3H</v>
           </cell>
         </row>
       </sheetData>
@@ -1259,7 +1262,7 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W59"/>
+  <dimension ref="A1:W62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
@@ -1269,10 +1272,10 @@
   <cols>
     <col min="1" max="1" width="5.85546875" style="5" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" style="5" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" style="5" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="96" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.85546875" style="5" customWidth="1"/>
     <col min="8" max="8" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
@@ -1353,7 +1356,7 @@
       </c>
       <c r="C3" s="48">
         <f>_xll.qlCalendarAdjust(_xll.qlIndexFixingCalendar(FirstIndex),_xll.qlSettingsEvaluationDate(ISERROR(Trigger)),"f")</f>
-        <v>41809</v>
+        <v>41810</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="17" t="e">
@@ -1370,7 +1373,7 @@
       </c>
       <c r="I3" s="45" t="str">
         <f>_xll.RData(H4,"LAST",,"FRQ:1S",,I4)</f>
-        <v>Updated at 17:23:41</v>
+        <v>Updated at 16:44:19</v>
       </c>
       <c r="J3" s="13"/>
       <c r="K3" s="4"/>
@@ -1395,7 +1398,7 @@
       </c>
       <c r="C4" s="40">
         <f>EvaluationDate</f>
-        <v>41809</v>
+        <v>41810</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="17" t="e">
@@ -1410,8 +1413,8 @@
       <c r="H4" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="44">
-        <v>124.515625</v>
+      <c r="I4" s="44" t="s">
+        <v>17</v>
       </c>
       <c r="J4" s="13"/>
       <c r="K4" s="4"/>
@@ -1434,17 +1437,17 @@
         <f>UPPER(Currency)&amp;"3M"</f>
         <v>CNH3M</v>
       </c>
-      <c r="C5" s="40" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="C5" s="40">
+        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D")</f>
+        <v>41814</v>
       </c>
       <c r="D5" s="16"/>
-      <c r="E5" s="17" t="e">
+      <c r="E5" s="17">
         <f>_xll.qlYieldTSDiscount(B5,C5,,Trigger)</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
       <c r="F5" s="18" t="str">
-        <f ca="1">IF(ISERROR(C5),_xll.ohRangeRetrieveError(C5),_xll.ohRangeRetrieveError(E5))</f>
+        <f>IF(ISERROR(C5),_xll.ohRangeRetrieveError(C5),_xll.ohRangeRetrieveError(E5))</f>
         <v/>
       </c>
       <c r="G5" s="52"/>
@@ -1453,7 +1456,7 @@
       </c>
       <c r="I5" s="20">
         <f>[1]!TriggerCounter</f>
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="J5" s="13"/>
       <c r="K5" s="4"/>
@@ -1475,7 +1478,7 @@
       <c r="B6" s="23"/>
       <c r="C6" s="41">
         <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-2D","Preceding")</f>
-        <v>41807</v>
+        <v>41808</v>
       </c>
       <c r="D6" s="24"/>
       <c r="E6" s="25" t="e">
@@ -1484,7 +1487,7 @@
       </c>
       <c r="F6" s="14" t="str">
         <f ca="1">IF(ISERROR(C6),_xll.ohRangeRetrieveError(C6),_xll.ohRangeRetrieveError(E6))</f>
-        <v>qlIndexFixing - Missing HiborSN Actual/365 (Fixed) fixing for June 17th, 2014</v>
+        <v>qlIndexFixing - Missing Hibor3M Actual/365 (Fixed) fixing for June 18th, 2014</v>
       </c>
       <c r="G6" s="52"/>
       <c r="H6" s="19" t="s">
@@ -1492,7 +1495,7 @@
       </c>
       <c r="I6" s="20">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>159</v>
+        <v>189</v>
       </c>
       <c r="J6" s="13"/>
       <c r="K6" s="4"/>
@@ -1514,7 +1517,7 @@
       <c r="B7" s="26"/>
       <c r="C7" s="42">
         <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-1D","Preceding")</f>
-        <v>41808</v>
+        <v>41809</v>
       </c>
       <c r="D7" s="35"/>
       <c r="E7" s="28" t="e">
@@ -1523,7 +1526,7 @@
       </c>
       <c r="F7" s="18" t="str">
         <f ca="1">IF(ISERROR(C7),_xll.ohRangeRetrieveError(C7),_xll.ohRangeRetrieveError(E7))</f>
-        <v>qlIndexFixing - Missing HiborSN Actual/365 (Fixed) fixing for June 18th, 2014</v>
+        <v>qlIndexFixing - Missing Hibor3M Actual/365 (Fixed) fixing for June 19th, 2014</v>
       </c>
       <c r="G7" s="52"/>
       <c r="H7" s="33" t="s">
@@ -1555,12 +1558,12 @@
       </c>
       <c r="C8" s="42">
         <f>EvaluationDate</f>
-        <v>41809</v>
+        <v>41810</v>
       </c>
       <c r="D8" s="27"/>
       <c r="E8" s="28">
         <f>_xll.qlIndexFixing(FirstIndex,C8)</f>
-        <v>3.0844999999999997E-2</v>
+        <v>2.9235323007457618E-2</v>
       </c>
       <c r="F8" s="18" t="str">
         <f>IF(ISERROR(C8),_xll.ohRangeRetrieveError(C8),_xll.ohRangeRetrieveError(E8))</f>
@@ -1597,13 +1600,13 @@
         <v>41988</v>
       </c>
       <c r="D9" s="30"/>
-      <c r="E9" s="31" t="e">
+      <c r="E9" s="31">
         <f>_xll.qlIndexFixing(FirstIndex,C9,TRUE)</f>
-        <v>#NUM!</v>
+        <v>2.64418785424386E-2</v>
       </c>
       <c r="F9" s="32" t="str">
-        <f ca="1">IF(ISERROR(C9),_xll.ohRangeRetrieveError(C9),_xll.ohRangeRetrieveError(E9))</f>
-        <v>qlIndexFixing - null term structure set to this instance of HiborSN Actual/365 (Fixed)</v>
+        <f>IF(ISERROR(C9),_xll.ohRangeRetrieveError(C9),_xll.ohRangeRetrieveError(E9))</f>
+        <v/>
       </c>
       <c r="G9" s="52"/>
       <c r="H9" s="21" t="s">
@@ -2692,6 +2695,11 @@
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
@@ -2712,6 +2720,11 @@
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
@@ -2732,6 +2745,14 @@
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
@@ -2749,6 +2770,15 @@
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
@@ -2764,6 +2794,16 @@
       <c r="W55" s="4"/>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
@@ -2779,6 +2819,16 @@
       <c r="W56" s="4"/>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A57" s="4"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
@@ -2794,6 +2844,16 @@
       <c r="W57" s="4"/>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A58" s="4"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
@@ -2809,6 +2869,16 @@
       <c r="W58" s="4"/>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
@@ -2822,6 +2892,81 @@
       <c r="U59" s="4"/>
       <c r="V59" s="4"/>
       <c r="W59" s="4"/>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
+      <c r="L60" s="4"/>
+      <c r="M60" s="4"/>
+      <c r="N60" s="4"/>
+      <c r="O60" s="4"/>
+      <c r="P60" s="4"/>
+      <c r="Q60" s="4"/>
+      <c r="R60" s="4"/>
+      <c r="S60" s="4"/>
+      <c r="T60" s="4"/>
+      <c r="U60" s="4"/>
+      <c r="V60" s="4"/>
+      <c r="W60" s="4"/>
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="4"/>
+      <c r="L61" s="4"/>
+      <c r="M61" s="4"/>
+      <c r="N61" s="4"/>
+      <c r="O61" s="4"/>
+      <c r="P61" s="4"/>
+      <c r="Q61" s="4"/>
+      <c r="R61" s="4"/>
+      <c r="S61" s="4"/>
+      <c r="T61" s="4"/>
+      <c r="U61" s="4"/>
+      <c r="V61" s="4"/>
+      <c r="W61" s="4"/>
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A62" s="4"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="4"/>
+      <c r="L62" s="4"/>
+      <c r="M62" s="4"/>
+      <c r="N62" s="4"/>
+      <c r="O62" s="4"/>
+      <c r="P62" s="4"/>
+      <c r="Q62" s="4"/>
+      <c r="R62" s="4"/>
+      <c r="S62" s="4"/>
+      <c r="T62" s="4"/>
+      <c r="U62" s="4"/>
+      <c r="V62" s="4"/>
+      <c r="W62" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>